<commit_message>
update to fix leakage computation and border adjustment computation for production taxes
</commit_message>
<xml_diff>
--- a/simulation_results/raw_data/energy_extraction_calculation.xlsx
+++ b/simulation_results/raw_data/energy_extraction_calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexdong/Desktop/Optimal-Unilateral-Carbon-Policy/simulation_results/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21745CFF-B4E8-424C-B1CC-317BE9657E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C27464F-2661-8944-9807-9FEFA4E562C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="1780" windowWidth="22520" windowHeight="16340" activeTab="2" xr2:uid="{8D74C7CE-2325-427A-8E43-F125F8FCCAF2}"/>
+    <workbookView xWindow="5540" yWindow="2560" windowWidth="22520" windowHeight="16340" activeTab="2" xr2:uid="{8D74C7CE-2325-427A-8E43-F125F8FCCAF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>L: Missing value; data exist but were not collected</t>
         </r>
@@ -63,7 +63,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>L: Missing value; data exist but were not collected</t>
         </r>
@@ -76,7 +76,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>L: Missing value; data exist but were not collected</t>
         </r>
@@ -276,7 +276,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -433,12 +433,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -453,6 +447,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -794,42 +794,42 @@
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="17"/>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="8" t="s">
+      <c r="G1" s="14"/>
+      <c r="H1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="8" t="s">
+      <c r="I1" s="14"/>
+      <c r="J1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="8" t="s">
+      <c r="K1" s="14"/>
+      <c r="L1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="9"/>
-      <c r="N1" s="8" t="s">
+      <c r="M1" s="14"/>
+      <c r="N1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="9"/>
-      <c r="P1" s="8" t="s">
+      <c r="O1" s="14"/>
+      <c r="P1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="8" t="s">
+      <c r="Q1" s="14"/>
+      <c r="R1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="9"/>
-      <c r="T1" s="8" t="s">
+      <c r="S1" s="14"/>
+      <c r="T1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="9"/>
+      <c r="U1" s="14"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -841,45 +841,45 @@
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="11"/>
-      <c r="L2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="11"/>
-      <c r="N2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="S2" s="11"/>
-      <c r="T2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="U2" s="11"/>
+      <c r="D2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="9"/>
+      <c r="J2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="9"/>
+      <c r="L2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="9"/>
+      <c r="N2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="9"/>
+      <c r="P2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" s="9"/>
+      <c r="T2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="U2" s="9"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -944,7 +944,7 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
@@ -1007,7 +1007,7 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
@@ -1070,7 +1070,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" s="13"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
@@ -1133,7 +1133,7 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
@@ -1196,7 +1196,7 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
@@ -1344,6 +1344,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="P2:Q2"/>
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="A3:A8"/>
@@ -1360,10 +1364,6 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="P2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1392,7 +1392,7 @@
       </c>
     </row>
     <row r="6" spans="2:11" ht="24" x14ac:dyDescent="0.2">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1426,7 +1426,7 @@
       </c>
     </row>
     <row r="7" spans="2:11" ht="24" x14ac:dyDescent="0.2">
-      <c r="B7" s="13"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
@@ -1450,7 +1450,7 @@
       </c>
     </row>
     <row r="8" spans="2:11" ht="36" x14ac:dyDescent="0.2">
-      <c r="B8" s="13"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
@@ -1470,7 +1470,7 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="13"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="3" t="s">
         <v>20</v>
       </c>
@@ -1486,7 +1486,7 @@
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="13"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="3" t="s">
         <v>21</v>
       </c>
@@ -1502,7 +1502,7 @@
       </c>
     </row>
     <row r="11" spans="2:11" ht="72" x14ac:dyDescent="0.2">
-      <c r="B11" s="13"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
@@ -1518,7 +1518,7 @@
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="13"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
@@ -1534,7 +1534,7 @@
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="13"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="3" t="s">
         <v>22</v>
       </c>
@@ -1550,7 +1550,7 @@
       </c>
     </row>
     <row r="14" spans="2:11" ht="24" x14ac:dyDescent="0.2">
-      <c r="B14" s="14"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="3" t="s">
         <v>31</v>
       </c>
@@ -1566,7 +1566,7 @@
       </c>
     </row>
     <row r="15" spans="2:11" ht="24" x14ac:dyDescent="0.2">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="10" t="s">
         <v>32</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1588,7 +1588,7 @@
       </c>
     </row>
     <row r="16" spans="2:11" ht="24" x14ac:dyDescent="0.2">
-      <c r="B16" s="13"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="3" t="s">
         <v>16</v>
       </c>
@@ -1604,7 +1604,7 @@
       </c>
     </row>
     <row r="17" spans="2:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="B17" s="13"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="3" t="s">
         <v>19</v>
       </c>
@@ -1620,7 +1620,7 @@
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="13"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="3" t="s">
         <v>20</v>
       </c>
@@ -1636,7 +1636,7 @@
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="13"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="3" t="s">
         <v>21</v>
       </c>
@@ -1652,7 +1652,7 @@
       </c>
     </row>
     <row r="20" spans="2:6" ht="72" x14ac:dyDescent="0.2">
-      <c r="B20" s="13"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="3" t="s">
         <v>29</v>
       </c>
@@ -1668,7 +1668,7 @@
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="13"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="3" t="s">
         <v>30</v>
       </c>
@@ -1684,7 +1684,7 @@
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="13"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="3" t="s">
         <v>22</v>
       </c>
@@ -1700,7 +1700,7 @@
       </c>
     </row>
     <row r="23" spans="2:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="B23" s="14"/>
+      <c r="B23" s="12"/>
       <c r="C23" s="3" t="s">
         <v>31</v>
       </c>
@@ -1728,15 +1728,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79B4F3F-0136-9E46-B81B-B90A105EC17F}">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.6640625" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -1947,11 +1951,11 @@
         <v>8.3616600077791592</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H3:H66" si="1">G10*0.92</f>
+        <f t="shared" ref="H10:H50" si="1">G10*0.92</f>
         <v>7.6927272071568265</v>
       </c>
       <c r="K10">
-        <f t="shared" ref="K3:K50" si="2">H10/1.0190249</f>
+        <f t="shared" ref="K10:K50" si="2">H10/1.0190249</f>
         <v>7.5491062163022971</v>
       </c>
     </row>

</xml_diff>